<commit_message>
implementado envio de mensagem
</commit_message>
<xml_diff>
--- a/datebase/contas.xlsx
+++ b/datebase/contas.xlsx
@@ -31,7 +31,7 @@
     <t xml:space="preserve">Enviados</t>
   </si>
   <si>
-    <t xml:space="preserve">emilson.sn1</t>
+    <t xml:space="preserve">emilson.sn</t>
   </si>
   <si>
     <t xml:space="preserve">emilson.sn2</t>
@@ -58,6 +58,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -245,10 +246,10 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.46"/>

</xml_diff>